<commit_message>
Add view booking and list of booking
</commit_message>
<xml_diff>
--- a/sc2002/src/main/resources/ApplicantList.xlsx
+++ b/sc2002/src/main/resources/ApplicantList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Chan\Documents\GitHub\SC2002\sc2002\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D24400A-EA84-4BE2-8A90-3D448FB7339B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384EB4E0-D057-41CA-96FB-5B08534DCB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3045" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6675" yWindow="3735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -399,7 +399,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +497,7 @@
         <v>17</v>
       </c>
       <c r="C6">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>

</xml_diff>